<commit_message>
initialize repository. video merger
</commit_message>
<xml_diff>
--- a/spreadsheets/spreadsheet1.xlsx
+++ b/spreadsheets/spreadsheet1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Python\General\VideoMerger\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Python\Freelances\VideoMerger\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9991F7-2583-424C-8FEC-E4173D21B577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77B1D46-617D-49E1-97AD-7528B9E231E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>videos/video3.mp4</t>
   </si>
   <si>
-    <t>videos/audio1.mp3</t>
-  </si>
-  <si>
     <t>output1</t>
   </si>
   <si>
@@ -56,6 +53,9 @@
   </si>
   <si>
     <t>output3</t>
+  </si>
+  <si>
+    <t>videos/audio0.mp3</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,10 +464,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -481,10 +481,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -498,10 +498,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>